<commit_message>
criado banco de dados
</commit_message>
<xml_diff>
--- a/Documentacao/Documentos App/ModelagemDeDaodos.xlsx
+++ b/Documentacao/Documentos App/ModelagemDeDaodos.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renato Nogueira\OneDrive\Área de Trabalho\ProjetoIntegrador\projetoIntegrador1\Documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renato Nogueira\OneDrive\Área de Trabalho\ProjetoIntegrador\projetoIntegrador1\Documentacao\Documentos App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15031E23-2E31-437D-932B-CA5F10210815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143C7CCE-D7C6-4313-9957-C1D70B2B8CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="56">
   <si>
     <t>USUARIO</t>
   </si>
@@ -48,9 +50,6 @@
     <t>ID (PK)</t>
   </si>
   <si>
-    <t>TIPO_USUARIO</t>
-  </si>
-  <si>
     <t>ONG</t>
   </si>
   <si>
@@ -63,24 +62,12 @@
     <t>SENHA</t>
   </si>
   <si>
-    <t>ID_TIPO_USUARIO (FK)</t>
-  </si>
-  <si>
     <t>DOCUMENTO</t>
   </si>
   <si>
-    <t>ID_PEDIDOS (FK)</t>
-  </si>
-  <si>
     <t>PRODUTO</t>
   </si>
   <si>
-    <t>QUANTIDADE_ESTOQUE</t>
-  </si>
-  <si>
-    <t>ID_USUARIO</t>
-  </si>
-  <si>
     <t>DATA_DE_VALIDADE</t>
   </si>
   <si>
@@ -100,6 +87,114 @@
   </si>
   <si>
     <t>PEDIDO</t>
+  </si>
+  <si>
+    <t>IDTIPO (PK)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>IDUSUARIO (PK)</t>
+  </si>
+  <si>
+    <t>ID_TIPO (FK)</t>
+  </si>
+  <si>
+    <t>ID_ESTOQUE</t>
+  </si>
+  <si>
+    <t>DESCRICAO</t>
+  </si>
+  <si>
+    <t>QUANTIDADE</t>
+  </si>
+  <si>
+    <t>IDPEDIDO</t>
+  </si>
+  <si>
+    <t>ID_PRODUTO_PEDIDO(FK)</t>
+  </si>
+  <si>
+    <t>ID_USUARIO (FK)</t>
+  </si>
+  <si>
+    <t>VALOR</t>
+  </si>
+  <si>
+    <t>PRODUTO_PEDIDO</t>
+  </si>
+  <si>
+    <t>IDPRODUTOPEDIDO</t>
+  </si>
+  <si>
+    <t>ID_PRODUTO (FK)</t>
+  </si>
+  <si>
+    <t>ESTOQUE</t>
+  </si>
+  <si>
+    <t>PRODUTO PEDIDO</t>
+  </si>
+  <si>
+    <t>IDUSUARIO</t>
+  </si>
+  <si>
+    <t>NÃO NULO</t>
+  </si>
+  <si>
+    <t>TEXTO</t>
+  </si>
+  <si>
+    <t>ÚNICO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> INTEIRO</t>
+  </si>
+  <si>
+    <t>INTEIRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTEIRO </t>
+  </si>
+  <si>
+    <t>IDESTOQUE</t>
+  </si>
+  <si>
+    <t>IDTIPO</t>
+  </si>
+  <si>
+    <t>INTERO</t>
+  </si>
+  <si>
+    <t>CHAVE ESTRANGEIRA</t>
+  </si>
+  <si>
+    <t>IDPRODUTO</t>
+  </si>
+  <si>
+    <t>DATA_VALIDADE</t>
+  </si>
+  <si>
+    <t>CHAVE PRIMARIA</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>DECIMAL</t>
+  </si>
+  <si>
+    <t>ID_ESTOQUE (FK)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDPEDIDO </t>
+  </si>
+  <si>
+    <t>IDPRODUTO_PEDIDO</t>
+  </si>
+  <si>
+    <t>ID_PEDIDO (FK)</t>
   </si>
 </sst>
 </file>
@@ -157,7 +252,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -205,14 +300,51 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right style="medium">
+      <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -222,7 +354,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -231,6 +363,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -242,12 +380,22 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -529,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C15:R32"/>
+  <dimension ref="C15:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView topLeftCell="H10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,106 +688,103 @@
     <col min="1" max="2" width="0" style="1" hidden="1" customWidth="1"/>
     <col min="3" max="7" width="9.109375" style="1" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="38.88671875" style="1" customWidth="1"/>
-    <col min="19" max="34" width="9.109375" style="1"/>
-    <col min="35" max="35" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="39" width="9.109375" style="1"/>
-    <col min="40" max="40" width="21.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="43" width="9.109375" style="1"/>
-    <col min="44" max="44" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="16384" width="9.109375" style="1"/>
+    <col min="11" max="11" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="32" width="9.109375" style="1"/>
+    <col min="33" max="33" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="37" width="9.109375" style="1"/>
+    <col min="38" max="38" width="21.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="41" width="9.109375" style="1"/>
+    <col min="42" max="42" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="15" spans="9:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="9:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I16" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="J16" s="7"/>
-    </row>
-    <row r="17" spans="9:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I17" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J17" s="8" t="s">
+      <c r="I16" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="9:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I18" s="3">
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="4" t="s">
         <v>1</v>
       </c>
+    </row>
+    <row r="18" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I18" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="J18" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="9:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I19" s="3">
         <v>2</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="9:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I20" s="3">
         <v>3</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="9:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="9:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I22" s="4" t="s">
+    <row r="22" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I22" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="6"/>
-    </row>
-    <row r="23" spans="9:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I23" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J23" s="8" t="s">
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+    </row>
+    <row r="23" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K23" s="8" t="s">
+      <c r="K23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="O23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L23" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="M23" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="N23" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="O23" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="P23" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="9:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -647,56 +792,58 @@
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-    </row>
-    <row r="26" spans="9:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="9:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I27" s="4" t="s">
+    </row>
+    <row r="27" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I27" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+    </row>
+    <row r="28" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M28" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
-      <c r="R27" s="5"/>
-    </row>
-    <row r="28" spans="9:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I28" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="K28" s="8" t="s">
+      <c r="N28" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L28" s="8" t="s">
+      <c r="O28" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M28" s="8" t="s">
+      <c r="P28" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N28" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O28" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="P28" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q28" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="R28" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="9:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q28" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="R28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="S28" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="9:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -705,26 +852,412 @@
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
-    </row>
-    <row r="31" spans="9:18" x14ac:dyDescent="0.3">
-      <c r="I31" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="9:18" x14ac:dyDescent="0.3">
-      <c r="I32" s="1" t="s">
-        <v>23</v>
+    </row>
+    <row r="33" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I33" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I37" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I38" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I22:P22"/>
-    <mergeCell ref="I27:R27"/>
+    <mergeCell ref="I22:O22"/>
+    <mergeCell ref="I27:S27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D4E034-23A4-4CE1-9A1F-DCEE9971446F}">
+  <dimension ref="E5:I29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31:I38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="4" width="8.88671875" style="10"/>
+    <col min="5" max="5" width="16.21875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E5" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E6" s="11"/>
+      <c r="F6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E7" s="11"/>
+      <c r="F7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E8" s="11"/>
+      <c r="F8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E9" s="11"/>
+      <c r="F9" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E10" s="11"/>
+      <c r="F10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E11" s="11"/>
+      <c r="F11" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E13" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E14" s="11"/>
+      <c r="F14" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E17" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E18" s="11"/>
+      <c r="F18" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E20" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E21" s="11"/>
+      <c r="F21" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E22" s="11"/>
+      <c r="F22" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E23" s="11"/>
+      <c r="F23" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E24" s="11"/>
+      <c r="F24" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E25" s="11"/>
+      <c r="F25" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E26" s="11"/>
+      <c r="F26" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E27" s="11"/>
+      <c r="F27" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E28" s="11"/>
+      <c r="F28" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E29" s="11"/>
+      <c r="F29" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E5:E11"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="E20:E29"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645EBA5E-DFA9-4009-B1EC-BCF8B24ADDF2}">
+  <dimension ref="I11:L18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10:M19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="7" width="8.88671875" style="10"/>
+    <col min="8" max="8" width="4.5546875" style="10" customWidth="1"/>
+    <col min="9" max="9" width="16.21875" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="18.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.21875" style="10" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="11" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I12" s="12"/>
+      <c r="J12" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12" s="18"/>
+    </row>
+    <row r="13" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I13" s="12"/>
+      <c r="J13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="L13" s="16"/>
+    </row>
+    <row r="15" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I15" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I16" s="12"/>
+      <c r="J16" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I17" s="12"/>
+      <c r="J17" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I18" s="12"/>
+      <c r="J18" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="I15:I18"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>